<commit_message>
Saving the corresponding LibreOffice file as an Excel file in 2-ipip-100_item-NEO5-20/ipip-100_items_NEO5-20.xlsx .
</commit_message>
<xml_diff>
--- a/questionnaires/2-ipip-100_item-NEO5-20/ipip-100_items_NEO5-20.xlsx
+++ b/questionnaires/2-ipip-100_item-NEO5-20/ipip-100_items_NEO5-20.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="IPIP 100 Item NEO5_20 Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Score Values for .csv" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="132">
   <si>
     <t xml:space="preserve">IPIP 100 Item Big Five Open Source Questionnaire</t>
   </si>
@@ -437,6 +438,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use right-click → Paste Special → Paste Special… to paste just the score here, then use File → Save As… to save that as a .csv file</t>
   </si>
 </sst>
 </file>
@@ -571,7 +575,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,6 +615,10 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -850,7 +858,7 @@
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -861,7 +869,7 @@
       <c r="H5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="10" t="n">
+      <c r="I5" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J5" s="0" t="n">
@@ -902,7 +910,7 @@
       <c r="H6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="10" t="n">
+      <c r="I6" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -943,7 +951,7 @@
       <c r="H7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="10" t="n">
+      <c r="I7" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J7" s="0" t="n">
@@ -984,7 +992,7 @@
       <c r="H8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="10" t="n">
+      <c r="I8" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J8" s="0" t="n">
@@ -1025,7 +1033,7 @@
       <c r="H9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="10" t="n">
+      <c r="I9" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J9" s="0" t="n">
@@ -1066,7 +1074,7 @@
       <c r="H10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="10" t="n">
+      <c r="I10" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J10" s="0" t="n">
@@ -1107,7 +1115,7 @@
       <c r="H11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="10" t="n">
+      <c r="I11" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J11" s="0" t="n">
@@ -1148,7 +1156,7 @@
       <c r="H12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="10" t="n">
+      <c r="I12" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J12" s="0" t="n">
@@ -1189,7 +1197,7 @@
       <c r="H13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="10" t="n">
+      <c r="I13" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J13" s="0" t="n">
@@ -1230,7 +1238,7 @@
       <c r="H14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="10" t="n">
+      <c r="I14" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J14" s="0" t="n">
@@ -1271,7 +1279,7 @@
       <c r="H15" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="10" t="n">
+      <c r="I15" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J15" s="0" t="n">
@@ -1312,7 +1320,7 @@
       <c r="H16" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="10" t="n">
+      <c r="I16" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J16" s="0" t="n">
@@ -1353,7 +1361,7 @@
       <c r="H17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="10" t="n">
+      <c r="I17" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J17" s="0" t="n">
@@ -1394,7 +1402,7 @@
       <c r="H18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="10" t="n">
+      <c r="I18" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J18" s="0" t="n">
@@ -1435,7 +1443,7 @@
       <c r="H19" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="10" t="n">
+      <c r="I19" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J19" s="0" t="n">
@@ -1476,7 +1484,7 @@
       <c r="H20" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="10" t="n">
+      <c r="I20" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J20" s="0" t="n">
@@ -1517,7 +1525,7 @@
       <c r="H21" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="10" t="n">
+      <c r="I21" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J21" s="0" t="n">
@@ -1558,7 +1566,7 @@
       <c r="H22" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="10" t="n">
+      <c r="I22" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J22" s="0" t="n">
@@ -1599,7 +1607,7 @@
       <c r="H23" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="10" t="n">
+      <c r="I23" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J23" s="0" t="n">
@@ -1640,7 +1648,7 @@
       <c r="H24" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="10" t="n">
+      <c r="I24" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J24" s="0" t="n">
@@ -1681,7 +1689,7 @@
       <c r="H25" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="10" t="n">
+      <c r="I25" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J25" s="0" t="n">
@@ -1722,7 +1730,7 @@
       <c r="H26" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="10" t="n">
+      <c r="I26" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J26" s="0" t="n">
@@ -1763,7 +1771,7 @@
       <c r="H27" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="10" t="n">
+      <c r="I27" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J27" s="0" t="n">
@@ -1804,7 +1812,7 @@
       <c r="H28" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="10" t="n">
+      <c r="I28" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J28" s="0" t="n">
@@ -1845,7 +1853,7 @@
       <c r="H29" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="10" t="n">
+      <c r="I29" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J29" s="0" t="n">
@@ -1886,7 +1894,7 @@
       <c r="H30" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="10" t="n">
+      <c r="I30" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J30" s="0" t="n">
@@ -1927,7 +1935,7 @@
       <c r="H31" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="10" t="n">
+      <c r="I31" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J31" s="0" t="n">
@@ -1968,7 +1976,7 @@
       <c r="H32" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="10" t="n">
+      <c r="I32" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J32" s="0" t="n">
@@ -2009,7 +2017,7 @@
       <c r="H33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I33" s="10" t="n">
+      <c r="I33" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J33" s="0" t="n">
@@ -2050,7 +2058,7 @@
       <c r="H34" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="10" t="n">
+      <c r="I34" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J34" s="0" t="n">
@@ -2091,7 +2099,7 @@
       <c r="H35" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="10" t="n">
+      <c r="I35" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J35" s="0" t="n">
@@ -2132,7 +2140,7 @@
       <c r="H36" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="10" t="n">
+      <c r="I36" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J36" s="0" t="n">
@@ -2173,7 +2181,7 @@
       <c r="H37" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I37" s="10" t="n">
+      <c r="I37" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J37" s="0" t="n">
@@ -2214,7 +2222,7 @@
       <c r="H38" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="10" t="n">
+      <c r="I38" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J38" s="0" t="n">
@@ -2255,7 +2263,7 @@
       <c r="H39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="10" t="n">
+      <c r="I39" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J39" s="0" t="n">
@@ -2296,7 +2304,7 @@
       <c r="H40" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="10" t="n">
+      <c r="I40" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J40" s="0" t="n">
@@ -2337,7 +2345,7 @@
       <c r="H41" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="10" t="n">
+      <c r="I41" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J41" s="0" t="n">
@@ -2378,7 +2386,7 @@
       <c r="H42" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="10" t="n">
+      <c r="I42" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J42" s="0" t="n">
@@ -2419,7 +2427,7 @@
       <c r="H43" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="10" t="n">
+      <c r="I43" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J43" s="0" t="n">
@@ -2460,7 +2468,7 @@
       <c r="H44" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I44" s="10" t="n">
+      <c r="I44" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J44" s="0" t="n">
@@ -2501,7 +2509,7 @@
       <c r="H45" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="10" t="n">
+      <c r="I45" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J45" s="0" t="n">
@@ -2542,7 +2550,7 @@
       <c r="H46" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I46" s="10" t="n">
+      <c r="I46" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J46" s="0" t="n">
@@ -2583,7 +2591,7 @@
       <c r="H47" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I47" s="10" t="n">
+      <c r="I47" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J47" s="0" t="n">
@@ -2624,7 +2632,7 @@
       <c r="H48" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I48" s="10" t="n">
+      <c r="I48" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J48" s="0" t="n">
@@ -2665,7 +2673,7 @@
       <c r="H49" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I49" s="10" t="n">
+      <c r="I49" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J49" s="0" t="n">
@@ -2706,7 +2714,7 @@
       <c r="H50" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I50" s="10" t="n">
+      <c r="I50" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J50" s="0" t="n">
@@ -2747,7 +2755,7 @@
       <c r="H51" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I51" s="10" t="n">
+      <c r="I51" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J51" s="0" t="n">
@@ -2788,7 +2796,7 @@
       <c r="H52" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="10" t="n">
+      <c r="I52" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J52" s="0" t="n">
@@ -2829,7 +2837,7 @@
       <c r="H53" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="10" t="n">
+      <c r="I53" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J53" s="0" t="n">
@@ -2870,7 +2878,7 @@
       <c r="H54" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I54" s="10" t="n">
+      <c r="I54" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J54" s="0" t="n">
@@ -2911,7 +2919,7 @@
       <c r="H55" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I55" s="10" t="n">
+      <c r="I55" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J55" s="0" t="n">
@@ -2952,7 +2960,7 @@
       <c r="H56" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I56" s="10" t="n">
+      <c r="I56" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J56" s="0" t="n">
@@ -2993,7 +3001,7 @@
       <c r="H57" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I57" s="10" t="n">
+      <c r="I57" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J57" s="0" t="n">
@@ -3034,7 +3042,7 @@
       <c r="H58" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I58" s="10" t="n">
+      <c r="I58" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J58" s="0" t="n">
@@ -3075,7 +3083,7 @@
       <c r="H59" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="10" t="n">
+      <c r="I59" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J59" s="0" t="n">
@@ -3116,7 +3124,7 @@
       <c r="H60" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I60" s="10" t="n">
+      <c r="I60" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J60" s="0" t="n">
@@ -3157,7 +3165,7 @@
       <c r="H61" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I61" s="10" t="n">
+      <c r="I61" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J61" s="0" t="n">
@@ -3198,7 +3206,7 @@
       <c r="H62" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I62" s="10" t="n">
+      <c r="I62" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J62" s="0" t="n">
@@ -3239,7 +3247,7 @@
       <c r="H63" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="10" t="n">
+      <c r="I63" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J63" s="0" t="n">
@@ -3280,7 +3288,7 @@
       <c r="H64" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I64" s="10" t="n">
+      <c r="I64" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J64" s="0" t="n">
@@ -3321,7 +3329,7 @@
       <c r="H65" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I65" s="10" t="n">
+      <c r="I65" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J65" s="0" t="n">
@@ -3362,7 +3370,7 @@
       <c r="H66" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I66" s="10" t="n">
+      <c r="I66" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J66" s="0" t="n">
@@ -3403,7 +3411,7 @@
       <c r="H67" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I67" s="10" t="n">
+      <c r="I67" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J67" s="0" t="n">
@@ -3444,7 +3452,7 @@
       <c r="H68" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I68" s="10" t="n">
+      <c r="I68" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J68" s="0" t="n">
@@ -3485,7 +3493,7 @@
       <c r="H69" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I69" s="10" t="n">
+      <c r="I69" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J69" s="0" t="n">
@@ -3526,7 +3534,7 @@
       <c r="H70" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I70" s="10" t="n">
+      <c r="I70" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J70" s="0" t="n">
@@ -3567,7 +3575,7 @@
       <c r="H71" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I71" s="10" t="n">
+      <c r="I71" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J71" s="0" t="n">
@@ -3608,7 +3616,7 @@
       <c r="H72" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I72" s="10" t="n">
+      <c r="I72" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J72" s="0" t="n">
@@ -3649,7 +3657,7 @@
       <c r="H73" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I73" s="10" t="n">
+      <c r="I73" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J73" s="0" t="n">
@@ -3690,7 +3698,7 @@
       <c r="H74" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I74" s="10" t="n">
+      <c r="I74" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J74" s="0" t="n">
@@ -3731,7 +3739,7 @@
       <c r="H75" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I75" s="10" t="n">
+      <c r="I75" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J75" s="0" t="n">
@@ -3772,7 +3780,7 @@
       <c r="H76" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I76" s="10" t="n">
+      <c r="I76" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J76" s="0" t="n">
@@ -3813,7 +3821,7 @@
       <c r="H77" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="10" t="n">
+      <c r="I77" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J77" s="0" t="n">
@@ -3854,7 +3862,7 @@
       <c r="H78" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I78" s="10" t="n">
+      <c r="I78" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J78" s="0" t="n">
@@ -3895,7 +3903,7 @@
       <c r="H79" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I79" s="10" t="n">
+      <c r="I79" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J79" s="0" t="n">
@@ -3936,7 +3944,7 @@
       <c r="H80" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I80" s="10" t="n">
+      <c r="I80" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J80" s="0" t="n">
@@ -3977,7 +3985,7 @@
       <c r="H81" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I81" s="10" t="n">
+      <c r="I81" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J81" s="0" t="n">
@@ -4018,7 +4026,7 @@
       <c r="H82" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="10" t="n">
+      <c r="I82" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J82" s="0" t="n">
@@ -4059,7 +4067,7 @@
       <c r="H83" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I83" s="10" t="n">
+      <c r="I83" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J83" s="0" t="n">
@@ -4100,7 +4108,7 @@
       <c r="H84" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I84" s="10" t="n">
+      <c r="I84" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J84" s="0" t="n">
@@ -4141,7 +4149,7 @@
       <c r="H85" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I85" s="10" t="n">
+      <c r="I85" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J85" s="0" t="n">
@@ -4182,7 +4190,7 @@
       <c r="H86" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I86" s="10" t="n">
+      <c r="I86" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J86" s="0" t="n">
@@ -4223,7 +4231,7 @@
       <c r="H87" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I87" s="10" t="n">
+      <c r="I87" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J87" s="0" t="n">
@@ -4264,7 +4272,7 @@
       <c r="H88" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I88" s="10" t="n">
+      <c r="I88" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J88" s="0" t="n">
@@ -4305,7 +4313,7 @@
       <c r="H89" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I89" s="10" t="n">
+      <c r="I89" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J89" s="0" t="n">
@@ -4346,7 +4354,7 @@
       <c r="H90" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I90" s="10" t="n">
+      <c r="I90" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J90" s="0" t="n">
@@ -4387,7 +4395,7 @@
       <c r="H91" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I91" s="10" t="n">
+      <c r="I91" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J91" s="0" t="n">
@@ -4428,7 +4436,7 @@
       <c r="H92" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I92" s="10" t="n">
+      <c r="I92" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J92" s="0" t="n">
@@ -4469,7 +4477,7 @@
       <c r="H93" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I93" s="10" t="n">
+      <c r="I93" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J93" s="0" t="n">
@@ -4510,7 +4518,7 @@
       <c r="H94" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I94" s="10" t="n">
+      <c r="I94" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J94" s="0" t="n">
@@ -4551,7 +4559,7 @@
       <c r="H95" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I95" s="10" t="n">
+      <c r="I95" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J95" s="0" t="n">
@@ -4592,7 +4600,7 @@
       <c r="H96" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I96" s="10" t="n">
+      <c r="I96" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J96" s="0" t="n">
@@ -4633,7 +4641,7 @@
       <c r="H97" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I97" s="10" t="n">
+      <c r="I97" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J97" s="0" t="n">
@@ -4674,7 +4682,7 @@
       <c r="H98" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I98" s="10" t="n">
+      <c r="I98" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J98" s="0" t="n">
@@ -4715,7 +4723,7 @@
       <c r="H99" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I99" s="10" t="n">
+      <c r="I99" s="11" t="n">
         <v>0.9</v>
       </c>
       <c r="J99" s="0" t="n">
@@ -4756,7 +4764,7 @@
       <c r="H100" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I100" s="10" t="n">
+      <c r="I100" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J100" s="0" t="n">
@@ -4797,7 +4805,7 @@
       <c r="H101" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I101" s="10" t="n">
+      <c r="I101" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J101" s="0" t="n">
@@ -4838,7 +4846,7 @@
       <c r="H102" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I102" s="10" t="n">
+      <c r="I102" s="11" t="n">
         <v>0.91</v>
       </c>
       <c r="J102" s="0" t="n">
@@ -4879,7 +4887,7 @@
       <c r="H103" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I103" s="10" t="n">
+      <c r="I103" s="11" t="n">
         <v>0.85</v>
       </c>
       <c r="J103" s="0" t="n">
@@ -4920,7 +4928,7 @@
       <c r="H104" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I104" s="10" t="n">
+      <c r="I104" s="11" t="n">
         <v>0.89</v>
       </c>
       <c r="J104" s="0" t="n">
@@ -4947,28 +4955,28 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="11" t="s">
+      <c r="A105" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
       <c r="G105" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H105" s="11" t="s">
+      <c r="H105" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
-      <c r="L105" s="11"/>
-      <c r="M105" s="11"/>
-      <c r="N105" s="11"/>
-      <c r="O105" s="11"/>
-      <c r="P105" s="11"/>
+      <c r="I105" s="12"/>
+      <c r="J105" s="12"/>
+      <c r="K105" s="12"/>
+      <c r="L105" s="12"/>
+      <c r="M105" s="12"/>
+      <c r="N105" s="12"/>
+      <c r="O105" s="12"/>
+      <c r="P105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2"/>
@@ -4981,7 +4989,7 @@
       <c r="O106" s="4"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="13" t="s">
         <v>121</v>
       </c>
       <c r="B107" s="2"/>
@@ -4994,7 +5002,7 @@
       <c r="O107" s="4"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="13"/>
+      <c r="A108" s="14"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -5025,8 +5033,8 @@
       <c r="O110" s="4"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="15"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -5035,16 +5043,16 @@
       <c r="O111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="15" t="s">
+      <c r="A112" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C112" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D112" s="14" t="s">
+      <c r="D112" s="15" t="s">
         <v>125</v>
       </c>
       <c r="E112" s="2"/>
@@ -5054,7 +5062,7 @@
       <c r="O112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="16" t="s">
+      <c r="A113" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B113" s="2" t="n">
@@ -5062,11 +5070,11 @@
         <v>0</v>
       </c>
       <c r="C113" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B113,10)</f>
-        <v>-10</v>
-      </c>
-      <c r="D113" s="17" t="str">
-        <f aca="false">IF(C113&lt;=20,"Very Low",IF(C113&lt;=40,"Low",IF(C113&lt;60,"Average",IF(C113&lt;80,"High","Very High"))))</f>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B113,20),5),4)</f>
+        <v>-25</v>
+      </c>
+      <c r="D113" s="18" t="str">
+        <f aca="false">IF(C113&lt;=20,"Very Low",IF(C113&lt;=36,"Low",IF(C113&lt;=46,"A Little Low",IF(C113&lt;=53,"Average",IF(C113&lt;=63,"A Little High",IF(C113&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="E113" s="2"/>
@@ -5076,7 +5084,7 @@
       <c r="O113" s="4"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="16" t="s">
+      <c r="A114" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B114" s="2" t="n">
@@ -5084,11 +5092,11 @@
         <v>0</v>
       </c>
       <c r="C114" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B114,10)</f>
-        <v>-10</v>
-      </c>
-      <c r="D114" s="17" t="str">
-        <f aca="false">IF(C114&lt;=20,"Very Low",IF(C114&lt;=40,"Low",IF(C114&lt;60,"Average",IF(C114&lt;80,"High","Very High"))))</f>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B114,20),5),4)</f>
+        <v>-25</v>
+      </c>
+      <c r="D114" s="18" t="str">
+        <f aca="false">IF(C114&lt;=20,"Very Low",IF(C114&lt;=36,"Low",IF(C114&lt;=46,"A Little Low",IF(C114&lt;=53,"Average",IF(C114&lt;=63,"A Little High",IF(C114&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="E114" s="2"/>
@@ -5098,7 +5106,7 @@
       <c r="O114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="16" t="s">
+      <c r="A115" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B115" s="2" t="n">
@@ -5106,11 +5114,11 @@
         <v>0</v>
       </c>
       <c r="C115" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B115,10)</f>
-        <v>-10</v>
-      </c>
-      <c r="D115" s="17" t="str">
-        <f aca="false">IF(C115&lt;=20,"Very Low",IF(C115&lt;=40,"Low",IF(C115&lt;60,"Average",IF(C115&lt;80,"High","Very High"))))</f>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B115,20),5),4)</f>
+        <v>-25</v>
+      </c>
+      <c r="D115" s="18" t="str">
+        <f aca="false">IF(C115&lt;=20,"Very Low",IF(C115&lt;=36,"Low",IF(C115&lt;=46,"A Little Low",IF(C115&lt;=53,"Average",IF(C115&lt;=63,"A Little High",IF(C115&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="E115" s="2"/>
@@ -5120,7 +5128,7 @@
       <c r="O115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="16" t="s">
+      <c r="A116" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B116" s="2" t="n">
@@ -5128,11 +5136,11 @@
         <v>0</v>
       </c>
       <c r="C116" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B116,10)</f>
-        <v>-10</v>
-      </c>
-      <c r="D116" s="17" t="str">
-        <f aca="false">IF(C116&lt;=20,"Very Low",IF(C116&lt;=40,"Low",IF(C116&lt;60,"Average",IF(C116&lt;80,"High","Very High"))))</f>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B116,20),5),4)</f>
+        <v>-25</v>
+      </c>
+      <c r="D116" s="18" t="str">
+        <f aca="false">IF(C116&lt;=20,"Very Low",IF(C116&lt;=36,"Low",IF(C116&lt;=46,"A Little Low",IF(C116&lt;=53,"Average",IF(C116&lt;=63,"A Little High",IF(C116&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="E116" s="2"/>
@@ -5142,7 +5150,7 @@
       <c r="O116" s="4"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="16" t="s">
+      <c r="A117" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B117" s="2" t="n">
@@ -5150,11 +5158,11 @@
         <v>0</v>
       </c>
       <c r="C117" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B117,10)</f>
-        <v>-10</v>
-      </c>
-      <c r="D117" s="17" t="str">
-        <f aca="false">IF(C117&lt;=20,"Very Low",IF(C117&lt;=40,"Low",IF(C117&lt;60,"Average",IF(C117&lt;80,"High","Very High"))))</f>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( B117,20),5),4)</f>
+        <v>-25</v>
+      </c>
+      <c r="D117" s="18" t="str">
+        <f aca="false">IF(C117&lt;=20,"Very Low",IF(C117&lt;=36,"Low",IF(C117&lt;=46,"A Little Low",IF(C117&lt;=53,"Average",IF(C117&lt;=63,"A Little High",IF(C117&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="E117" s="2"/>
@@ -5171,14 +5179,14 @@
       <c r="O118" s="4"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="18"/>
+      <c r="A125" s="19"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="18" t="s">
+      <c r="A126" s="19" t="s">
         <v>126</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -5821,4 +5829,33 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>